<commit_message>
Ajout du cahier des charges - arborescence - périmétre fonctionel
</commit_message>
<xml_diff>
--- a/Documentation/01b_Diagramme_de_Gantt.xlsx
+++ b/Documentation/01b_Diagramme_de_Gantt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Fichiers\Cours\BTS02_Efficom_2019_2020\Document_BTS\M2L_NoteDeFrais\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Fichiers\Cours\BTS02_Efficom_2019_2020\Document_BTS\M2L_NoteDeFrais\M2L_note_de_frais\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="822" documentId="11_B40CAD6F1578B032D4B1CE7B373DD4416449EE2A" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1A7CC832-38F9-4DF9-8E7D-5AA3D0B6F376}"/>
+  <xr:revisionPtr revIDLastSave="835" documentId="11_B40CAD6F1578B032D4B1CE7B373DD4416449EE2A" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9F2EDBAB-66A6-4F9A-B286-3D8848B4414F}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -922,7 +922,7 @@
   <dimension ref="A1:AK1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="E3" s="15">
         <f>(E4+E5)/2</f>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F3" s="16"/>
       <c r="G3" s="17" t="s">
@@ -1171,7 +1171,7 @@
       </c>
       <c r="H3" s="51">
         <f>$E$3</f>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="S3" s="19"/>
       <c r="T3" s="19"/>
@@ -1208,7 +1208,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="25">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>33</v>
@@ -1218,7 +1218,7 @@
       </c>
       <c r="H4" s="52">
         <f>$E$4</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I4" s="52"/>
       <c r="J4" s="52"/>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="E6" s="29">
         <f>(E7+E8)/2</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="17" t="s">
@@ -1336,7 +1336,7 @@
       <c r="L6" s="52"/>
       <c r="M6" s="55">
         <f>$E$6</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N6" s="55"/>
       <c r="O6" s="55"/>
@@ -1376,7 +1376,7 @@
         <v>63</v>
       </c>
       <c r="E7" s="25">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F7" s="24" t="s">
         <v>37</v>
@@ -1391,7 +1391,7 @@
       <c r="L7" s="52"/>
       <c r="M7" s="55">
         <f>$E$7</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N7" s="55"/>
       <c r="O7" s="55"/>
@@ -1431,7 +1431,7 @@
         <v>63</v>
       </c>
       <c r="E8" s="25">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F8" s="24" t="s">
         <v>37</v>
@@ -1446,7 +1446,7 @@
       <c r="L8" s="52"/>
       <c r="M8" s="55">
         <f>$E$8</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N8" s="55"/>
       <c r="O8" s="55"/>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="E9" s="15">
         <f>(E10+E11+E12+E13+E14)/5</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="17" t="s">
@@ -1495,7 +1495,7 @@
       </c>
       <c r="H9" s="55">
         <f>E9</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I9" s="55"/>
       <c r="J9" s="55"/>
@@ -1540,7 +1540,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="25">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>37</v>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="H10" s="52">
         <f>E10</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I10" s="52"/>
       <c r="J10" s="52"/>
@@ -1595,7 +1595,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="25">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>38</v>
@@ -1605,7 +1605,7 @@
       </c>
       <c r="H11" s="52">
         <f>E11</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I11" s="52"/>
       <c r="J11" s="52"/>
@@ -1650,7 +1650,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="25">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F12" s="24" t="s">
         <v>38</v>
@@ -1660,7 +1660,7 @@
       </c>
       <c r="H12" s="52">
         <f>E12</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I12" s="52"/>
       <c r="J12" s="52"/>
@@ -1705,7 +1705,7 @@
         <v>56</v>
       </c>
       <c r="E13" s="25">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>37</v>
@@ -1721,7 +1721,7 @@
       <c r="M13" s="52"/>
       <c r="N13" s="55">
         <f>E13</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O13" s="55"/>
       <c r="P13" s="55"/>
@@ -1760,7 +1760,7 @@
         <v>56</v>
       </c>
       <c r="E14" s="25">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F14" s="24" t="s">
         <v>37</v>
@@ -1776,7 +1776,7 @@
       <c r="M14" s="52"/>
       <c r="N14" s="55">
         <f>E14</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O14" s="55"/>
       <c r="P14" s="55"/>
@@ -1816,7 +1816,7 @@
       </c>
       <c r="E15" s="37">
         <f>(E16+E17+E18+E19)/4</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F15" s="38"/>
       <c r="G15" s="39" t="s">
@@ -1824,7 +1824,7 @@
       </c>
       <c r="I15" s="55">
         <f>$E$15</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J15" s="55"/>
       <c r="K15" s="55"/>
@@ -1870,7 +1870,7 @@
         <v>35</v>
       </c>
       <c r="E16" s="25">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F16" s="24" t="s">
         <v>37</v>
@@ -1881,7 +1881,7 @@
       <c r="H16" s="52"/>
       <c r="I16" s="55">
         <f>$E$16</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J16" s="55"/>
       <c r="K16" s="55"/>
@@ -1925,7 +1925,7 @@
         <v>35</v>
       </c>
       <c r="E17" s="25">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F17" s="24" t="s">
         <v>37</v>
@@ -1936,7 +1936,7 @@
       <c r="H17" s="52"/>
       <c r="I17" s="55">
         <f>$E$17</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J17" s="55"/>
       <c r="K17" s="55"/>
@@ -1980,7 +1980,7 @@
         <v>21</v>
       </c>
       <c r="E18" s="25">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>37</v>
@@ -1996,7 +1996,7 @@
       <c r="M18" s="52"/>
       <c r="N18" s="55">
         <f>$E$18</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O18" s="55"/>
       <c r="P18" s="55"/>
@@ -2035,7 +2035,7 @@
         <v>14</v>
       </c>
       <c r="E19" s="25">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>37</v>
@@ -2057,7 +2057,7 @@
       <c r="S19" s="52"/>
       <c r="T19" s="55">
         <f>E19</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="U19" s="55"/>
       <c r="V19" s="52"/>
@@ -2089,7 +2089,7 @@
       </c>
       <c r="E20" s="37">
         <f>(E21)/1</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F20" s="38"/>
       <c r="G20" s="54" t="s">
@@ -2111,7 +2111,7 @@
       <c r="U20" s="52"/>
       <c r="V20" s="52">
         <f>E20</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="W20" s="52"/>
       <c r="X20" s="52"/>
@@ -2144,7 +2144,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="25">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F21" s="24" t="s">
         <v>37</v>
@@ -2168,7 +2168,7 @@
       <c r="U21" s="52"/>
       <c r="V21" s="52">
         <f>E21</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="W21" s="52"/>
       <c r="X21" s="52"/>
@@ -39369,6 +39369,10 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="T19:U19"/>
+    <mergeCell ref="N14:U14"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="M6:U6"/>
     <mergeCell ref="I15:U15"/>
     <mergeCell ref="I16:M16"/>
     <mergeCell ref="I17:M17"/>
@@ -39376,10 +39380,6 @@
     <mergeCell ref="M8:U8"/>
     <mergeCell ref="H9:U9"/>
     <mergeCell ref="N13:U13"/>
-    <mergeCell ref="T19:U19"/>
-    <mergeCell ref="N14:U14"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="M6:U6"/>
   </mergeCells>
   <conditionalFormatting sqref="Z4:Z21">
     <cfRule type="dataBar" priority="36">

</xml_diff>